<commit_message>
Modificacion del word y excel
</commit_message>
<xml_diff>
--- a/Plan_Direccionamiento.xlsx
+++ b/Plan_Direccionamiento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Caso de estudio-REDES\Caso-de-estudio-redes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD103E9A-90CD-4F74-9D28-26DB358DD05B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B19C64-038F-467E-B38F-CF9B182101F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C1A70FEA-A176-4610-89D6-5E8630C399F7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
   <si>
     <t xml:space="preserve">SEDES </t>
   </si>
@@ -63,13 +63,163 @@
   </si>
   <si>
     <t>Descripción</t>
+  </si>
+  <si>
+    <t>Primera dirección</t>
+  </si>
+  <si>
+    <t>Última dirección</t>
+  </si>
+  <si>
+    <t>Grandes</t>
+  </si>
+  <si>
+    <t>Pequeñas</t>
+  </si>
+  <si>
+    <t>Machala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuenca </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Babahoyo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esmeraldas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portoviejo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ibarra </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ambato </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riobamba </t>
+  </si>
+  <si>
+    <t>Latacunga</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Santa Elena</t>
+  </si>
+  <si>
+    <t>SUCURSALES</t>
+  </si>
+  <si>
+    <t>Manta</t>
+  </si>
+  <si>
+    <t>Bahía</t>
+  </si>
+  <si>
+    <t>Chone</t>
+  </si>
+  <si>
+    <t>Jipijapa</t>
+  </si>
+  <si>
+    <t>Milagro</t>
+  </si>
+  <si>
+    <t>El Triunfo</t>
+  </si>
+  <si>
+    <t>Durán</t>
+  </si>
+  <si>
+    <t>Naranjal</t>
+  </si>
+  <si>
+    <t>Daule</t>
+  </si>
+  <si>
+    <t>Pasaje</t>
+  </si>
+  <si>
+    <t>El Guabo</t>
+  </si>
+  <si>
+    <t>Santa Rosa</t>
+  </si>
+  <si>
+    <t>Huaquillas</t>
+  </si>
+  <si>
+    <t>Salinas</t>
+  </si>
+  <si>
+    <t>La Libertad</t>
+  </si>
+  <si>
+    <t>Quevedo</t>
+  </si>
+  <si>
+    <t>Valencia</t>
+  </si>
+  <si>
+    <t>Ventanas</t>
+  </si>
+  <si>
+    <t>Vinces</t>
+  </si>
+  <si>
+    <t>Montalvo</t>
+  </si>
+  <si>
+    <t>San Lorenzo</t>
+  </si>
+  <si>
+    <t>Muisne</t>
+  </si>
+  <si>
+    <t>Quinindé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atacames </t>
+  </si>
+  <si>
+    <t>Gualeco</t>
+  </si>
+  <si>
+    <t>Chordeleg</t>
+  </si>
+  <si>
+    <t>Girón</t>
+  </si>
+  <si>
+    <t>Paute</t>
+  </si>
+  <si>
+    <t>Otavalo</t>
+  </si>
+  <si>
+    <t>Atuntaqui</t>
+  </si>
+  <si>
+    <t>Cotacachi</t>
+  </si>
+  <si>
+    <t>Mejía</t>
+  </si>
+  <si>
+    <t>Cayambe</t>
+  </si>
+  <si>
+    <t>Sangolqui</t>
+  </si>
+  <si>
+    <t>Machachí</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,8 +234,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,8 +267,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -178,40 +347,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -527,121 +735,528 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3ECA57C-C0C6-48F2-B4A3-4DC99C95754C}">
-  <dimension ref="A2:G8"/>
+  <dimension ref="A2:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="8" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="F5" s="8"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="F6" s="8"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="3" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="F7" s="8"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="17"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="17"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="17"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="4:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D33" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="4:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D34" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="4:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="4:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D36" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="4:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D38" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="4:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D39" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D40" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="4:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D43" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="4:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D44" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="4:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D45" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="4:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D46" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="4:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D47" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="4:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D48" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
+  <mergeCells count="16">
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="D12:F12"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>